<commit_message>
Added AccountTransaction Child Class
</commit_message>
<xml_diff>
--- a/Banking Mini Project/bankingEnv/data/BankingData.xlsx
+++ b/Banking Mini Project/bankingEnv/data/BankingData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renga/Documents/SpringBoard Data Engineering Course/SpringBoard/Banking Mini Project/bankingEnv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23486356-9958-DA45-A35E-CDAC1E83BBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17CF32D-A67E-924E-8E3D-F9391CE656E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3860" yWindow="500" windowWidth="28040" windowHeight="16420" activeTab="2" xr2:uid="{53CE078C-3FFB-5942-8CD9-E853A9DE31EF}"/>
+    <workbookView xWindow="5220" yWindow="1320" windowWidth="28040" windowHeight="16420" activeTab="2" xr2:uid="{53CE078C-3FFB-5942-8CD9-E853A9DE31EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="159">
   <si>
     <t>Id</t>
   </si>
@@ -85,24 +85,18 @@
     <t>HandlesBusinessLoan</t>
   </si>
   <si>
-    <t>False</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
     <t>CustomerType</t>
   </si>
   <si>
     <t>PersonalBankerId</t>
   </si>
   <si>
+    <t>ServiceId</t>
+  </si>
+  <si>
     <t>MinimumBalance</t>
   </si>
   <si>
-    <t>Fees</t>
-  </si>
-  <si>
     <t>WithdrawalLimitPerDay</t>
   </si>
   <si>
@@ -289,57 +283,15 @@
     <t>AS0001</t>
   </si>
   <si>
-    <t>{
-  "Currency":"USD",
-  "MonthlyFee":4,
-  "ExcessWithdrawalsOrTransferOutside":3,
-  "ATMWithdrawalFeeOutNetwork":2.5,
-  "AllowedATMWithdrawals":5,
-  "AllowedTransactions":7,
-  "OverDraftCoverageFee":35,
-  "EarlyAccountClosing":25,
-  "EarlyAccountClosingPeriodInDays":30,
-  "InsufficientFunds":35
-}</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
-    <t>{
-  "Currency":"USD",
-  "MonthlyFee":10,
-  "ExcessWithdrawalsOrTransferOutside":3,
-  "ATMWithdrawalFeeOutNetwork":2.5,
-  "AllowedATMWithdrawals":5,
-  "AllowedTransactions":7,
-  "OverDraftCoverageFee":35,
-  "EarlyAccountClosing":25,
-  "EarlyAccountClosingPeriodInDays":30,
-  "InsufficientFunds":35
-}</t>
-  </si>
-  <si>
     <t>AS0002</t>
   </si>
   <si>
     <t>250</t>
   </si>
   <si>
-    <t>{
-  "Currency":"USD",
-  "MonthlyFee":0,
-  "ExcessWithdrawalsOrTransferOutside":3,
-  "ATMWithdrawalFeeOutNetwork":2.5,
-  "AllowedATMWithdrawals":5,
-  "AllowedTransactions":7,
-  "OverDraftCoverageFee":35,
-  "EarlyAccountClosing":25,
-  "EarlyAccountClosingPeriodInDays":30,
-  "InsufficientFunds":35
-}</t>
-  </si>
-  <si>
     <t>AS0003</t>
   </si>
   <si>
@@ -358,34 +310,6 @@
     <t>AS0006</t>
   </si>
   <si>
-    <t>{
-  "Currency":"USD",
-  "MonthlyFee":10,
-  "ExcessWithdrawalsOrTransferOutside":3,
-  "ATMWithdrawalFeeOutNetwork":2.5,
-  "AllowedATMWithdrawals":2,
-  "AllowedTransactions":3,
-  "OverDraftCoverageFee":35,
-  "EarlyAccountClosing":25,
-  "EarlyAccountClosingPeriodInDays":30,
-  "InsufficientFunds":35
-}</t>
-  </si>
-  <si>
-    <t>{
-  "Currency":"USD",
-  "MonthlyFee":0,
-  "ExcessWithdrawalsOrTransferOutside":3,
-  "ATMWithdrawalFeeOutNetwork":2.5,
-  "AllowedATMWithdrawals":2,
-  "AllowedTransactions":3,
-  "OverDraftCoverageFee":35,
-  "EarlyAccountClosing":25,
-  "EarlyAccountClosingPeriodInDays":30,
-  "InsufficientFunds":35
-}</t>
-  </si>
-  <si>
     <t>LS0001</t>
   </si>
   <si>
@@ -413,24 +337,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>{
-   "Currency":"USD",
-   "LoanCostPercent":0.02,
-   "LateFeePercent":1,
-   "PrepaymentFeePercent":0.01,
-   "PrepaymentTermInMonths":3
-}</t>
-  </si>
-  <si>
-    <t>{
-   "Currency":"USD",
-   "LoanCostPercent":0.025,
-   "LateFeePercent":1.1,
-   "PrepaymentFeePercent":0.01,
-   "PrepaymentTermInMonths":3
-}</t>
-  </si>
-  <si>
     <t>LS0002</t>
   </si>
   <si>
@@ -443,24 +349,6 @@
     <t>150000</t>
   </si>
   <si>
-    <t>{
-   "Currency":"USD",
-   "LoanCostPercent":0.02,
-   "LateFeePercent":1,
-   "PrepaymentFeePercent":0.01,
-   "PrepaymentTermInMonths":60
-}</t>
-  </si>
-  <si>
-    <t>{
-   "Currency":"USD",
-   "LoanCostPercent":0.025,
-   "LateFeePercent":1.1,
-   "PrepaymentFeePercent":0.01,
-   "PrepaymentTermInMonths":60
-}</t>
-  </si>
-  <si>
     <t>400000</t>
   </si>
   <si>
@@ -491,30 +379,12 @@
     <t>24</t>
   </si>
   <si>
-    <t>{
-   "Currency":"USD",
-   "LoanCostPercent":0.02,
-   "LateFeePercent":1,
-   "PrepaymentFeePercent":0.01,
-   "PrepaymentTermInMonths":12
-}</t>
-  </si>
-  <si>
     <t>100000</t>
   </si>
   <si>
     <t>36</t>
   </si>
   <si>
-    <t>{
-   "Currency":"USD",
-   "LoanCostPercent":0.025,
-   "LateFeePercent":1.1,
-   "PrepaymentFeePercent":0.01,
-   "PrepaymentTermInMonths":12
-}</t>
-  </si>
-  <si>
     <t>CS0001</t>
   </si>
   <si>
@@ -524,14 +394,6 @@
     <t>12</t>
   </si>
   <si>
-    <t>{
- "Currency":"USD",
- "YearlyFee":0,
- "YearlyFeeMinimumCreditLimit":500,
- "MinimumCreditScore":0
-}</t>
-  </si>
-  <si>
     <t>CS0002</t>
   </si>
   <si>
@@ -544,36 +406,9 @@
     <t>MasterCard</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>{
- "Currency":"USD",
- "YearlyFee":15,
- "YearlyFeeMinimumCreditLimit":10000,
- "MinimumCreditScore":400
-}</t>
-  </si>
-  <si>
-    <t>{
- "Currency":"USD",
- "YearlyFee":30,
- "YearlyFeeMinimumCreditLimit":20000,
- "MinimumCreditScore":600
-}</t>
-  </si>
-  <si>
     <t>20</t>
   </si>
   <si>
-    <t>{
- "Currency":"USD",
- "YearlyFee":60,
- "YearlyFeeMinimumCreditLimit":32000,
- "MinimumCreditScore":700
-}</t>
-  </si>
-  <si>
     <t>AddressLine2</t>
   </si>
   <si>
@@ -628,34 +463,61 @@
     <t>AccountDetailId</t>
   </si>
   <si>
-    <t>D00000001</t>
-  </si>
-  <si>
-    <t>D00000002</t>
-  </si>
-  <si>
-    <t>D00000003</t>
-  </si>
-  <si>
-    <t>D00000004</t>
-  </si>
-  <si>
-    <t>D00000005</t>
-  </si>
-  <si>
-    <t>D00000006</t>
-  </si>
-  <si>
-    <t>D00000007</t>
-  </si>
-  <si>
-    <t>D00000008</t>
-  </si>
-  <si>
-    <t>D00000009</t>
-  </si>
-  <si>
-    <t>D00000010</t>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>0.0001</t>
+  </si>
+  <si>
+    <t>0.0002</t>
+  </si>
+  <si>
+    <t>0.0003</t>
+  </si>
+  <si>
+    <t>0.001</t>
+  </si>
+  <si>
+    <t>0.002</t>
+  </si>
+  <si>
+    <t>MonthlyFees</t>
+  </si>
+  <si>
+    <t>LoanCostPercentage</t>
+  </si>
+  <si>
+    <t>PrepaymentFeePercentage</t>
+  </si>
+  <si>
+    <t>MinimumMonthsBeforePrepayment</t>
+  </si>
+  <si>
+    <t>MinimumCreditScore</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>YearlyFees</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>FreeTransactionCountPerMonth</t>
+  </si>
+  <si>
+    <t>TransactionFees</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +911,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:O2"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1084,7 +946,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1119,222 +981,222 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" t="s">
         <v>36</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="H2">
         <v>30339</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="N2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="F3" t="s">
         <v>44</v>
       </c>
-      <c r="D3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H3">
         <v>30041</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>15</v>
+        <v>156</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>15</v>
+        <v>156</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>15</v>
+        <v>156</v>
       </c>
       <c r="N3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H4">
         <v>30320</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="N4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" t="s">
-        <v>54</v>
-      </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H5">
         <v>30339</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>15</v>
+        <v>156</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="N5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="F6" t="s">
         <v>56</v>
       </c>
-      <c r="D6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" t="s">
-        <v>58</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H6">
         <v>30024</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>15</v>
+        <v>156</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>15</v>
+        <v>156</v>
       </c>
       <c r="N6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1368,7 +1230,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1380,7 +1242,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1395,13 +1257,13 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>11</v>
@@ -1412,198 +1274,198 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="H2">
         <v>30339</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H3">
         <v>30041</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H4">
         <v>30320</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H5">
         <v>30339</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H6">
         <v>30024</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J6" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="L6" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1614,234 +1476,299 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5294827-AD73-C045-9A5F-9E780EE8C8A6}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="64" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="64" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="D2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="I2">
+        <v>10000</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="306" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="I3">
+        <v>10000</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="6"/>
+    </row>
+    <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="E4" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I4">
+        <v>15000</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>84</v>
       </c>
-      <c r="F2">
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I5">
+        <v>25000</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I6">
         <v>10000</v>
       </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="5"/>
-    </row>
-    <row r="3" spans="1:12" ht="306" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="J6" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3">
+      <c r="F7" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="I7">
         <v>10000</v>
       </c>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:12" ht="306" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="F4">
-        <v>10000</v>
-      </c>
-      <c r="G4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="306" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F5">
-        <v>10000</v>
-      </c>
-      <c r="G5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" s="5"/>
-    </row>
-    <row r="6" spans="1:12" ht="306" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="F6">
-        <v>10000</v>
-      </c>
-      <c r="G6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="5"/>
-    </row>
-    <row r="7" spans="1:12" ht="306" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7">
-        <v>10000</v>
-      </c>
-      <c r="G7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L7" s="5"/>
+      <c r="J7" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1850,10 +1777,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8A9F79-3B49-5C40-A490-3D6F93CA8129}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1865,237 +1792,279 @@
     <col min="5" max="5" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.5" customWidth="1"/>
+    <col min="8" max="10" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C2">
         <v>1000</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="I2" s="9">
+        <v>3</v>
+      </c>
+      <c r="J2" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="119" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>107</v>
-      </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C3">
         <v>10000</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" s="9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I3" s="9">
+        <v>3</v>
+      </c>
+      <c r="J3" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>103</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-    </row>
-    <row r="4" spans="1:12" ht="119" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>114</v>
-      </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C4">
         <v>75000</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-    </row>
-    <row r="5" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+      <c r="H4" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="I4" s="9">
+        <v>60</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C5">
         <v>150000</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-    </row>
-    <row r="6" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="H5" s="9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I5" s="9">
+        <v>60</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C6">
         <v>1000</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="I6" s="9">
+        <v>12</v>
+      </c>
+      <c r="J6" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C7">
         <v>10000</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>30</v>
+        <v>95</v>
+      </c>
+      <c r="H7" s="9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I7" s="9">
+        <v>12</v>
+      </c>
+      <c r="J7" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2105,194 +2074,183 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57974CD4-C9D0-FD46-B924-3F91A35F3DEC}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="2"/>
-    <col min="6" max="6" width="20.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.83203125" customWidth="1"/>
-    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>152</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>154</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="170" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C2">
         <v>500</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="I2">
+        <v>92</v>
+      </c>
+      <c r="G2" s="9">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>100</v>
       </c>
+      <c r="I2" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="J2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="187" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C3">
         <v>15000</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>83</v>
+      <c r="D3">
+        <v>400</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>135</v>
+        <v>80</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="I3">
+        <v>116</v>
+      </c>
+      <c r="G3" s="9">
+        <v>15</v>
+      </c>
+      <c r="H3">
         <v>1000</v>
       </c>
+      <c r="I3" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="J3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="187" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="C4">
         <v>30000</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>83</v>
+      <c r="D4">
+        <v>600</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>129</v>
+        <v>80</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="I4">
+        <v>153</v>
+      </c>
+      <c r="G4" s="9">
+        <v>30</v>
+      </c>
+      <c r="H4">
         <v>5000</v>
       </c>
+      <c r="I4" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="J4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="187" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="C5">
         <v>45000</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>83</v>
+      <c r="D5">
+        <v>700</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="I5">
+        <v>121</v>
+      </c>
+      <c r="G5" s="9">
+        <v>60</v>
+      </c>
+      <c r="H5">
         <v>10000</v>
       </c>
+      <c r="I5" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="J5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2302,157 +2260,178 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EBC3DB-7AFA-C548-9172-806268290870}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>146</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2">
+        <v>500</v>
+      </c>
+      <c r="F2" s="10">
+        <v>10000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3">
+        <v>430</v>
+      </c>
+      <c r="F3" s="10">
+        <v>5000</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>61</v>
       </c>
-      <c r="B2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2">
-        <v>500</v>
-      </c>
-      <c r="E2" s="10">
-        <v>10000</v>
-      </c>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4">
+        <v>720</v>
+      </c>
+      <c r="F4" s="10">
+        <v>25000</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>62</v>
       </c>
-      <c r="B3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3">
-        <v>430</v>
-      </c>
-      <c r="E3" s="10">
-        <v>5000</v>
-      </c>
-      <c r="F3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5">
+        <v>655</v>
+      </c>
+      <c r="F5" s="10">
+        <v>30000</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>63</v>
       </c>
-      <c r="B4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4">
-        <v>655</v>
-      </c>
-      <c r="E4" s="10">
-        <v>25000</v>
-      </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5">
-        <v>720</v>
-      </c>
-      <c r="E5" s="10">
-        <v>30000</v>
-      </c>
-      <c r="F5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>65</v>
-      </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6">
-        <v>300</v>
-      </c>
-      <c r="E6" s="10">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6">
+        <v>760</v>
+      </c>
+      <c r="F6" s="10">
         <v>50000</v>
       </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2464,7 +2443,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD3FC9F7-F25E-7E43-A058-F8C408391786}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2477,16 +2458,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>11</v>
@@ -2496,178 +2477,203 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>158</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
+        <v>129</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
       </c>
       <c r="D2" s="10">
         <v>10000</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>159</v>
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>130</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
       </c>
       <c r="D3" s="10">
         <v>5000</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>160</v>
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>131</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
       </c>
       <c r="D4" s="10">
         <v>25000</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>161</v>
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>132</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
       </c>
       <c r="D5" s="10">
         <v>30000</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>162</v>
+      <c r="A6">
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>133</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
       </c>
       <c r="D6" s="10">
         <v>50000</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>163</v>
+      <c r="A7">
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="C7" s="10">
         <v>200</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>164</v>
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
-      </c>
-      <c r="C8" s="10"/>
+        <v>130</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0</v>
+      </c>
       <c r="D8" s="10">
         <v>400</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>165</v>
+      <c r="A9">
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="C9" s="10">
         <v>1000</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="10">
+        <v>0</v>
+      </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>166</v>
+      <c r="A10">
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
-      </c>
-      <c r="C10" s="10"/>
+        <v>132</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0</v>
+      </c>
       <c r="D10" s="10">
         <v>2000</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>167</v>
+      <c r="A11">
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="C11" s="10">
         <v>5000</v>
       </c>
-      <c r="D11" s="10"/>
+      <c r="D11" s="10">
+        <v>0</v>
+      </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated AccountTransaction Child Class
</commit_message>
<xml_diff>
--- a/Banking Mini Project/bankingEnv/data/BankingData.xlsx
+++ b/Banking Mini Project/bankingEnv/data/BankingData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renga/Documents/SpringBoard Data Engineering Course/SpringBoard/Banking Mini Project/bankingEnv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23486356-9958-DA45-A35E-CDAC1E83BBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17CF32D-A67E-924E-8E3D-F9391CE656E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3860" yWindow="500" windowWidth="28040" windowHeight="16420" activeTab="2" xr2:uid="{53CE078C-3FFB-5942-8CD9-E853A9DE31EF}"/>
+    <workbookView xWindow="5220" yWindow="1320" windowWidth="28040" windowHeight="16420" activeTab="2" xr2:uid="{53CE078C-3FFB-5942-8CD9-E853A9DE31EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="159">
   <si>
     <t>Id</t>
   </si>
@@ -85,24 +85,18 @@
     <t>HandlesBusinessLoan</t>
   </si>
   <si>
-    <t>False</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
     <t>CustomerType</t>
   </si>
   <si>
     <t>PersonalBankerId</t>
   </si>
   <si>
+    <t>ServiceId</t>
+  </si>
+  <si>
     <t>MinimumBalance</t>
   </si>
   <si>
-    <t>Fees</t>
-  </si>
-  <si>
     <t>WithdrawalLimitPerDay</t>
   </si>
   <si>
@@ -289,57 +283,15 @@
     <t>AS0001</t>
   </si>
   <si>
-    <t>{
-  "Currency":"USD",
-  "MonthlyFee":4,
-  "ExcessWithdrawalsOrTransferOutside":3,
-  "ATMWithdrawalFeeOutNetwork":2.5,
-  "AllowedATMWithdrawals":5,
-  "AllowedTransactions":7,
-  "OverDraftCoverageFee":35,
-  "EarlyAccountClosing":25,
-  "EarlyAccountClosingPeriodInDays":30,
-  "InsufficientFunds":35
-}</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
-    <t>{
-  "Currency":"USD",
-  "MonthlyFee":10,
-  "ExcessWithdrawalsOrTransferOutside":3,
-  "ATMWithdrawalFeeOutNetwork":2.5,
-  "AllowedATMWithdrawals":5,
-  "AllowedTransactions":7,
-  "OverDraftCoverageFee":35,
-  "EarlyAccountClosing":25,
-  "EarlyAccountClosingPeriodInDays":30,
-  "InsufficientFunds":35
-}</t>
-  </si>
-  <si>
     <t>AS0002</t>
   </si>
   <si>
     <t>250</t>
   </si>
   <si>
-    <t>{
-  "Currency":"USD",
-  "MonthlyFee":0,
-  "ExcessWithdrawalsOrTransferOutside":3,
-  "ATMWithdrawalFeeOutNetwork":2.5,
-  "AllowedATMWithdrawals":5,
-  "AllowedTransactions":7,
-  "OverDraftCoverageFee":35,
-  "EarlyAccountClosing":25,
-  "EarlyAccountClosingPeriodInDays":30,
-  "InsufficientFunds":35
-}</t>
-  </si>
-  <si>
     <t>AS0003</t>
   </si>
   <si>
@@ -358,34 +310,6 @@
     <t>AS0006</t>
   </si>
   <si>
-    <t>{
-  "Currency":"USD",
-  "MonthlyFee":10,
-  "ExcessWithdrawalsOrTransferOutside":3,
-  "ATMWithdrawalFeeOutNetwork":2.5,
-  "AllowedATMWithdrawals":2,
-  "AllowedTransactions":3,
-  "OverDraftCoverageFee":35,
-  "EarlyAccountClosing":25,
-  "EarlyAccountClosingPeriodInDays":30,
-  "InsufficientFunds":35
-}</t>
-  </si>
-  <si>
-    <t>{
-  "Currency":"USD",
-  "MonthlyFee":0,
-  "ExcessWithdrawalsOrTransferOutside":3,
-  "ATMWithdrawalFeeOutNetwork":2.5,
-  "AllowedATMWithdrawals":2,
-  "AllowedTransactions":3,
-  "OverDraftCoverageFee":35,
-  "EarlyAccountClosing":25,
-  "EarlyAccountClosingPeriodInDays":30,
-  "InsufficientFunds":35
-}</t>
-  </si>
-  <si>
     <t>LS0001</t>
   </si>
   <si>
@@ -413,24 +337,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>{
-   "Currency":"USD",
-   "LoanCostPercent":0.02,
-   "LateFeePercent":1,
-   "PrepaymentFeePercent":0.01,
-   "PrepaymentTermInMonths":3
-}</t>
-  </si>
-  <si>
-    <t>{
-   "Currency":"USD",
-   "LoanCostPercent":0.025,
-   "LateFeePercent":1.1,
-   "PrepaymentFeePercent":0.01,
-   "PrepaymentTermInMonths":3
-}</t>
-  </si>
-  <si>
     <t>LS0002</t>
   </si>
   <si>
@@ -443,24 +349,6 @@
     <t>150000</t>
   </si>
   <si>
-    <t>{
-   "Currency":"USD",
-   "LoanCostPercent":0.02,
-   "LateFeePercent":1,
-   "PrepaymentFeePercent":0.01,
-   "PrepaymentTermInMonths":60
-}</t>
-  </si>
-  <si>
-    <t>{
-   "Currency":"USD",
-   "LoanCostPercent":0.025,
-   "LateFeePercent":1.1,
-   "PrepaymentFeePercent":0.01,
-   "PrepaymentTermInMonths":60
-}</t>
-  </si>
-  <si>
     <t>400000</t>
   </si>
   <si>
@@ -491,30 +379,12 @@
     <t>24</t>
   </si>
   <si>
-    <t>{
-   "Currency":"USD",
-   "LoanCostPercent":0.02,
-   "LateFeePercent":1,
-   "PrepaymentFeePercent":0.01,
-   "PrepaymentTermInMonths":12
-}</t>
-  </si>
-  <si>
     <t>100000</t>
   </si>
   <si>
     <t>36</t>
   </si>
   <si>
-    <t>{
-   "Currency":"USD",
-   "LoanCostPercent":0.025,
-   "LateFeePercent":1.1,
-   "PrepaymentFeePercent":0.01,
-   "PrepaymentTermInMonths":12
-}</t>
-  </si>
-  <si>
     <t>CS0001</t>
   </si>
   <si>
@@ -524,14 +394,6 @@
     <t>12</t>
   </si>
   <si>
-    <t>{
- "Currency":"USD",
- "YearlyFee":0,
- "YearlyFeeMinimumCreditLimit":500,
- "MinimumCreditScore":0
-}</t>
-  </si>
-  <si>
     <t>CS0002</t>
   </si>
   <si>
@@ -544,36 +406,9 @@
     <t>MasterCard</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>{
- "Currency":"USD",
- "YearlyFee":15,
- "YearlyFeeMinimumCreditLimit":10000,
- "MinimumCreditScore":400
-}</t>
-  </si>
-  <si>
-    <t>{
- "Currency":"USD",
- "YearlyFee":30,
- "YearlyFeeMinimumCreditLimit":20000,
- "MinimumCreditScore":600
-}</t>
-  </si>
-  <si>
     <t>20</t>
   </si>
   <si>
-    <t>{
- "Currency":"USD",
- "YearlyFee":60,
- "YearlyFeeMinimumCreditLimit":32000,
- "MinimumCreditScore":700
-}</t>
-  </si>
-  <si>
     <t>AddressLine2</t>
   </si>
   <si>
@@ -628,34 +463,61 @@
     <t>AccountDetailId</t>
   </si>
   <si>
-    <t>D00000001</t>
-  </si>
-  <si>
-    <t>D00000002</t>
-  </si>
-  <si>
-    <t>D00000003</t>
-  </si>
-  <si>
-    <t>D00000004</t>
-  </si>
-  <si>
-    <t>D00000005</t>
-  </si>
-  <si>
-    <t>D00000006</t>
-  </si>
-  <si>
-    <t>D00000007</t>
-  </si>
-  <si>
-    <t>D00000008</t>
-  </si>
-  <si>
-    <t>D00000009</t>
-  </si>
-  <si>
-    <t>D00000010</t>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>0.0001</t>
+  </si>
+  <si>
+    <t>0.0002</t>
+  </si>
+  <si>
+    <t>0.0003</t>
+  </si>
+  <si>
+    <t>0.001</t>
+  </si>
+  <si>
+    <t>0.002</t>
+  </si>
+  <si>
+    <t>MonthlyFees</t>
+  </si>
+  <si>
+    <t>LoanCostPercentage</t>
+  </si>
+  <si>
+    <t>PrepaymentFeePercentage</t>
+  </si>
+  <si>
+    <t>MinimumMonthsBeforePrepayment</t>
+  </si>
+  <si>
+    <t>MinimumCreditScore</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>YearlyFees</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>FreeTransactionCountPerMonth</t>
+  </si>
+  <si>
+    <t>TransactionFees</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +911,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:O2"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1084,7 +946,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1119,222 +981,222 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" t="s">
         <v>36</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="H2">
         <v>30339</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="N2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="F3" t="s">
         <v>44</v>
       </c>
-      <c r="D3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H3">
         <v>30041</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>15</v>
+        <v>156</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>15</v>
+        <v>156</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>15</v>
+        <v>156</v>
       </c>
       <c r="N3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H4">
         <v>30320</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="N4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" t="s">
-        <v>54</v>
-      </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H5">
         <v>30339</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>15</v>
+        <v>156</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="N5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="F6" t="s">
         <v>56</v>
       </c>
-      <c r="D6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" t="s">
-        <v>58</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H6">
         <v>30024</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>15</v>
+        <v>156</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>15</v>
+        <v>156</v>
       </c>
       <c r="N6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1368,7 +1230,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1380,7 +1242,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1395,13 +1257,13 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>11</v>
@@ -1412,198 +1274,198 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="H2">
         <v>30339</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H3">
         <v>30041</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H4">
         <v>30320</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H5">
         <v>30339</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H6">
         <v>30024</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J6" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="L6" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1614,234 +1476,299 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5294827-AD73-C045-9A5F-9E780EE8C8A6}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="64" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="64" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="D2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="I2">
+        <v>10000</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="306" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="I3">
+        <v>10000</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="6"/>
+    </row>
+    <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="E4" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I4">
+        <v>15000</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>84</v>
       </c>
-      <c r="F2">
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I5">
+        <v>25000</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I6">
         <v>10000</v>
       </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="5"/>
-    </row>
-    <row r="3" spans="1:12" ht="306" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="J6" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3">
+      <c r="F7" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="I7">
         <v>10000</v>
       </c>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:12" ht="306" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="F4">
-        <v>10000</v>
-      </c>
-      <c r="G4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="306" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F5">
-        <v>10000</v>
-      </c>
-      <c r="G5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" s="5"/>
-    </row>
-    <row r="6" spans="1:12" ht="306" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="F6">
-        <v>10000</v>
-      </c>
-      <c r="G6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="5"/>
-    </row>
-    <row r="7" spans="1:12" ht="306" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7">
-        <v>10000</v>
-      </c>
-      <c r="G7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L7" s="5"/>
+      <c r="J7" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1850,10 +1777,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8A9F79-3B49-5C40-A490-3D6F93CA8129}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1865,237 +1792,279 @@
     <col min="5" max="5" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.5" customWidth="1"/>
+    <col min="8" max="10" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C2">
         <v>1000</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="I2" s="9">
+        <v>3</v>
+      </c>
+      <c r="J2" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="119" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>107</v>
-      </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C3">
         <v>10000</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" s="9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I3" s="9">
+        <v>3</v>
+      </c>
+      <c r="J3" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>103</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-    </row>
-    <row r="4" spans="1:12" ht="119" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>114</v>
-      </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C4">
         <v>75000</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-    </row>
-    <row r="5" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+      <c r="H4" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="I4" s="9">
+        <v>60</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C5">
         <v>150000</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-    </row>
-    <row r="6" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="H5" s="9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I5" s="9">
+        <v>60</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C6">
         <v>1000</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="I6" s="9">
+        <v>12</v>
+      </c>
+      <c r="J6" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C7">
         <v>10000</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>30</v>
+        <v>95</v>
+      </c>
+      <c r="H7" s="9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I7" s="9">
+        <v>12</v>
+      </c>
+      <c r="J7" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2105,194 +2074,183 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57974CD4-C9D0-FD46-B924-3F91A35F3DEC}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="2"/>
-    <col min="6" max="6" width="20.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.83203125" customWidth="1"/>
-    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>152</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>154</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="170" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C2">
         <v>500</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="I2">
+        <v>92</v>
+      </c>
+      <c r="G2" s="9">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>100</v>
       </c>
+      <c r="I2" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="J2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="187" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C3">
         <v>15000</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>83</v>
+      <c r="D3">
+        <v>400</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>135</v>
+        <v>80</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="I3">
+        <v>116</v>
+      </c>
+      <c r="G3" s="9">
+        <v>15</v>
+      </c>
+      <c r="H3">
         <v>1000</v>
       </c>
+      <c r="I3" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="J3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="187" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="C4">
         <v>30000</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>83</v>
+      <c r="D4">
+        <v>600</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>129</v>
+        <v>80</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="I4">
+        <v>153</v>
+      </c>
+      <c r="G4" s="9">
+        <v>30</v>
+      </c>
+      <c r="H4">
         <v>5000</v>
       </c>
+      <c r="I4" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="J4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="187" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="C5">
         <v>45000</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>83</v>
+      <c r="D5">
+        <v>700</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="I5">
+        <v>121</v>
+      </c>
+      <c r="G5" s="9">
+        <v>60</v>
+      </c>
+      <c r="H5">
         <v>10000</v>
       </c>
+      <c r="I5" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="J5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2302,157 +2260,178 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EBC3DB-7AFA-C548-9172-806268290870}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>146</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2">
+        <v>500</v>
+      </c>
+      <c r="F2" s="10">
+        <v>10000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3">
+        <v>430</v>
+      </c>
+      <c r="F3" s="10">
+        <v>5000</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>61</v>
       </c>
-      <c r="B2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2">
-        <v>500</v>
-      </c>
-      <c r="E2" s="10">
-        <v>10000</v>
-      </c>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4">
+        <v>720</v>
+      </c>
+      <c r="F4" s="10">
+        <v>25000</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>62</v>
       </c>
-      <c r="B3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3">
-        <v>430</v>
-      </c>
-      <c r="E3" s="10">
-        <v>5000</v>
-      </c>
-      <c r="F3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5">
+        <v>655</v>
+      </c>
+      <c r="F5" s="10">
+        <v>30000</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>63</v>
       </c>
-      <c r="B4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4">
-        <v>655</v>
-      </c>
-      <c r="E4" s="10">
-        <v>25000</v>
-      </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5">
-        <v>720</v>
-      </c>
-      <c r="E5" s="10">
-        <v>30000</v>
-      </c>
-      <c r="F5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>65</v>
-      </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6">
-        <v>300</v>
-      </c>
-      <c r="E6" s="10">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6">
+        <v>760</v>
+      </c>
+      <c r="F6" s="10">
         <v>50000</v>
       </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2464,7 +2443,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD3FC9F7-F25E-7E43-A058-F8C408391786}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2477,16 +2458,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>11</v>
@@ -2496,178 +2477,203 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>158</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
+        <v>129</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
       </c>
       <c r="D2" s="10">
         <v>10000</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>159</v>
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>130</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
       </c>
       <c r="D3" s="10">
         <v>5000</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>160</v>
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>131</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
       </c>
       <c r="D4" s="10">
         <v>25000</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>161</v>
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>132</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
       </c>
       <c r="D5" s="10">
         <v>30000</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>162</v>
+      <c r="A6">
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>133</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
       </c>
       <c r="D6" s="10">
         <v>50000</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>163</v>
+      <c r="A7">
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="C7" s="10">
         <v>200</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>164</v>
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
-      </c>
-      <c r="C8" s="10"/>
+        <v>130</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0</v>
+      </c>
       <c r="D8" s="10">
         <v>400</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>165</v>
+      <c r="A9">
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="C9" s="10">
         <v>1000</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="10">
+        <v>0</v>
+      </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>166</v>
+      <c r="A10">
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
-      </c>
-      <c r="C10" s="10"/>
+        <v>132</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0</v>
+      </c>
       <c r="D10" s="10">
         <v>2000</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>167</v>
+      <c r="A11">
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="C11" s="10">
         <v>5000</v>
       </c>
-      <c r="D11" s="10"/>
+      <c r="D11" s="10">
+        <v>0</v>
+      </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Account Transaction Class
</commit_message>
<xml_diff>
--- a/Banking Mini Project/bankingEnv/data/BankingData.xlsx
+++ b/Banking Mini Project/bankingEnv/data/BankingData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renga/Documents/SpringBoard Data Engineering Course/SpringBoard/Banking Mini Project/bankingEnv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17CF32D-A67E-924E-8E3D-F9391CE656E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C79378-2C82-C74D-B04A-948EAE8DFFC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="1320" windowWidth="28040" windowHeight="16420" activeTab="2" xr2:uid="{53CE078C-3FFB-5942-8CD9-E853A9DE31EF}"/>
+    <workbookView xWindow="5220" yWindow="1320" windowWidth="28040" windowHeight="16420" activeTab="5" xr2:uid="{53CE078C-3FFB-5942-8CD9-E853A9DE31EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -1478,8 +1478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5294827-AD73-C045-9A5F-9E780EE8C8A6}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2262,8 +2262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EBC3DB-7AFA-C548-9172-806268290870}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2344,7 +2344,7 @@
         <v>81</v>
       </c>
       <c r="E3">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="F3" s="10">
         <v>5000</v>

</xml_diff>